<commit_message>
bulk upload template excel modified
</commit_message>
<xml_diff>
--- a/public/excel/bulk_order_template.xlsx
+++ b/public/excel/bulk_order_template.xlsx
@@ -133,7 +133,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,7 +419,7 @@
   <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -426,7 +428,7 @@
     <col min="2" max="2" width="23.625" customWidth="1"/>
     <col min="3" max="3" width="22.375" customWidth="1"/>
     <col min="4" max="4" width="20.875" customWidth="1"/>
-    <col min="5" max="5" width="42.25" customWidth="1"/>
+    <col min="5" max="5" width="46.125" customWidth="1"/>
     <col min="6" max="6" width="17.5" customWidth="1"/>
     <col min="7" max="7" width="22.75" customWidth="1"/>
     <col min="8" max="8" width="17.375" customWidth="1"/>
@@ -495,53 +497,53 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
+      <c r="G2" s="1">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1">
         <v>5</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="1">
         <v>101</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="1">
         <v>4</v>
       </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="M2">
+      <c r="K2" s="1">
+        <v>1</v>
+      </c>
+      <c r="L2" s="1">
+        <v>1</v>
+      </c>
+      <c r="M2" s="1">
         <v>500</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="O2">
-        <v>1</v>
-      </c>
-      <c r="P2" t="s">
+      <c r="O2" s="1">
+        <v>1</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Q2">
+      <c r="Q2" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new bulk order template
</commit_message>
<xml_diff>
--- a/public/excel/bulk_order_template.xlsx
+++ b/public/excel/bulk_order_template.xlsx
@@ -1,30 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MY WORKS\BorakExpress\Borak-Express\public\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amitbiswas/Documents/Ext Project/Borak-Express/public/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EC36A817-8131-9A46-A009-9F54F407B399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16020" tabRatio="500"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16080" xr2:uid="{7B009823-284E-AB46-9554-59F9222BAD90}"/>
   </bookViews>
   <sheets>
-    <sheet name="bulk_order_template" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>sending_type</t>
   </si>
@@ -41,15 +51,15 @@
     <t>address</t>
   </si>
   <si>
+    <t>landmarks</t>
+  </si>
+  <si>
     <t>recipient_city</t>
   </si>
   <si>
     <t>recipient_area</t>
   </si>
   <si>
-    <t>landmarks</t>
-  </si>
-  <si>
     <t>product_id</t>
   </si>
   <si>
@@ -77,28 +87,19 @@
     <t>payment_method</t>
   </si>
   <si>
-    <t>01917720168</t>
-  </si>
-  <si>
     <t>Mr Akhtar U Ahmed</t>
   </si>
   <si>
     <t>H-106/2, bou bazar, shah ali bag,mirpur-1,dhaka-1216</t>
   </si>
   <si>
-    <t>2021-04-24</t>
-  </si>
-  <si>
     <t>delivery safely plz</t>
-  </si>
-  <si>
-    <t>01921307315</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -128,18 +129,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -197,9 +195,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian Light"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -227,14 +225,31 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -262,6 +277,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -413,36 +445,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4FA739D-7FB4-CD41-AC4A-F2CEE7A4FC71}">
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.75" customWidth="1"/>
-    <col min="2" max="2" width="23.625" customWidth="1"/>
-    <col min="3" max="3" width="22.375" customWidth="1"/>
-    <col min="4" max="4" width="20.875" customWidth="1"/>
-    <col min="5" max="5" width="42.25" customWidth="1"/>
-    <col min="6" max="6" width="17.5" customWidth="1"/>
-    <col min="7" max="7" width="22.75" customWidth="1"/>
-    <col min="8" max="8" width="17.375" customWidth="1"/>
-    <col min="9" max="9" width="16.75" customWidth="1"/>
-    <col min="10" max="10" width="21.5" customWidth="1"/>
-    <col min="11" max="11" width="19.375" customWidth="1"/>
-    <col min="12" max="12" width="23.75" customWidth="1"/>
-    <col min="13" max="14" width="21.75" customWidth="1"/>
-    <col min="15" max="15" width="24.375" customWidth="1"/>
-    <col min="16" max="16" width="20.625" customWidth="1"/>
-    <col min="17" max="17" width="18.5" customWidth="1"/>
-    <col min="18" max="18" width="16.875" customWidth="1"/>
-    <col min="19" max="19" width="26.5" customWidth="1"/>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="46.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -459,13 +490,13 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
         <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
       </c>
       <c r="I1" t="s">
         <v>8</v>
@@ -495,58 +526,55 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1917720168</v>
+      </c>
+      <c r="C2">
+        <v>1921307315</v>
+      </c>
+      <c r="D2" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>18</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>5</v>
+      </c>
+      <c r="H2">
+        <v>101</v>
+      </c>
+      <c r="I2">
+        <v>4</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>500</v>
+      </c>
+      <c r="M2" s="1">
+        <v>44310</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2" t="s">
         <v>19</v>
       </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>5</v>
-      </c>
-      <c r="I2">
-        <v>101</v>
-      </c>
-      <c r="J2">
-        <v>4</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="M2">
-        <v>500</v>
-      </c>
-      <c r="N2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O2">
-        <v>1</v>
-      </c>
-      <c r="P2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
+      <c r="P2">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
home page design change and add public tracking page
</commit_message>
<xml_diff>
--- a/public/excel/bulk_order_template.xlsx
+++ b/public/excel/bulk_order_template.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amitbiswas/Documents/Ext Project/Borak-Express/public/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MY WORKS\BorakExpress\Borak-Express\public\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EC36A817-8131-9A46-A009-9F54F407B399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16080" xr2:uid="{7B009823-284E-AB46-9554-59F9222BAD90}"/>
+    <workbookView xWindow="375" yWindow="465" windowWidth="28035" windowHeight="16080"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>sending_type</t>
   </si>
@@ -94,12 +93,18 @@
   </si>
   <si>
     <t>delivery safely plz</t>
+  </si>
+  <si>
+    <t>01917720168</t>
+  </si>
+  <si>
+    <t>01921307315</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -129,9 +134,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,35 +452,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4FA739D-7FB4-CD41-AC4A-F2CEE7A4FC71}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="46.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="46.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.75" customWidth="1"/>
+    <col min="16" max="16" width="22.875" customWidth="1"/>
+    <col min="17" max="17" width="15.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -526,15 +533,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>1917720168</v>
-      </c>
-      <c r="C2">
-        <v>1921307315</v>
+      <c r="B2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="D2" t="s">
         <v>17</v>
@@ -561,22 +568,26 @@
         <v>1</v>
       </c>
       <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2" s="3">
         <v>500</v>
       </c>
-      <c r="M2" s="1">
+      <c r="N2" s="1">
         <v>44310</v>
       </c>
-      <c r="N2">
-        <v>1</v>
-      </c>
-      <c r="O2" t="s">
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2" t="s">
         <v>19</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>